<commit_message>
Updating documentation and refactoring classes
Updating documentation and refactoring classes
</commit_message>
<xml_diff>
--- a/docs/Projeto.xlsx
+++ b/docs/Projeto.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Projetos\HovinJS\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
   </bookViews>
@@ -17,14 +12,14 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
   <si>
     <t>Basics</t>
   </si>
@@ -191,9 +186,6 @@
     <t>Versão</t>
   </si>
   <si>
-    <t>Requisitos mínimos</t>
-  </si>
-  <si>
     <t>Ivehicle</t>
   </si>
   <si>
@@ -203,23 +195,71 @@
     <t>Core</t>
   </si>
   <si>
-    <t>Criar e herdar objetos, fazer merge de objetos, adicionar e remover eventos, parse JSONe converter para String</t>
-  </si>
-  <si>
     <t>Converter Graus para Radianos, converter Radianos para Graus</t>
   </si>
   <si>
     <t>Somar, Subtrair, Multiplicar, Dividir, Clonar e Serializar</t>
   </si>
   <si>
-    <t xml:space="preserve">Criar novo por tamanho e ângulo, </t>
+    <t>Funções</t>
+  </si>
+  <si>
+    <t>Criar novo por tamanho e ângulo, tamanho, tamanho ao quadrado, normalizar, ângulo, rotação, ângulo entre dois vetores, normalizar e retornar novo</t>
+  </si>
+  <si>
+    <t>Atributos</t>
+  </si>
+  <si>
+    <t>x, y</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>width, height</t>
+  </si>
+  <si>
+    <t>herdar Point2</t>
+  </si>
+  <si>
+    <t>position, size</t>
+  </si>
+  <si>
+    <t>Escrita</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>Criar e herdar objetos, fazer merge de objetos, adicionar e remover eventos, parse JSON e converter para String</t>
+  </si>
+  <si>
+    <t>Gerar número 0 a 1, inteiro de 0 a max, número de 0 a max, número de min a max, inteiro min a max</t>
+  </si>
+  <si>
+    <t>ConsoleHJS</t>
+  </si>
+  <si>
+    <t>default, options</t>
+  </si>
+  <si>
+    <t>Criar, criar estilo, debug, debug linha nova, esconder, limpar</t>
+  </si>
+  <si>
+    <t>id, size, path, file, isLoaded</t>
+  </si>
+  <si>
+    <t>Retorna o objeto Image, tamanho, get de largura e altura, se está carregado ou não, função de desenho padrão, clonar, serializar</t>
+  </si>
+  <si>
+    <t>Clonar e serializar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,7 +282,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -315,6 +355,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -343,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -400,6 +446,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -472,7 +527,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -504,10 +559,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,7 +593,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -715,23 +768,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="18" style="3" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="107.140625" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="32.140625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="104.7109375" style="5" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="6" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
@@ -742,126 +797,184 @@
         <v>54</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="2" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C2" s="7">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="C2" s="20">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="20">
+        <v>1</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="20">
+        <v>1</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="20">
+        <v>1</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="2" customFormat="1">
       <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="20">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="C7" s="20">
+        <v>1</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="C8" s="20">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1">
+      <c r="A9" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C9" s="7">
-        <v>3</v>
-      </c>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="D9" s="7"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="22"/>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1">
+      <c r="A10" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C10" s="7">
-        <v>3</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1" ht="30">
       <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
@@ -871,431 +984,528 @@
       <c r="C11" s="7">
         <v>1</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>9</v>
+      <c r="D11" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11" s="22"/>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1">
+      <c r="A12" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="C12" s="7">
-        <v>2</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="D12" s="7"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1">
+      <c r="A13" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C13" s="7">
-        <v>2</v>
-      </c>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="11" t="s">
-        <v>13</v>
+        <v>1</v>
+      </c>
+      <c r="D13" s="7"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1">
+      <c r="A14" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="C14" s="7">
         <v>1</v>
       </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>13</v>
+      <c r="D14" s="7"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1">
+      <c r="A15" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C15" s="7">
         <v>1</v>
       </c>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>13</v>
+      <c r="D15" s="7"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="22"/>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1">
+      <c r="A16" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C16" s="7">
         <v>1</v>
       </c>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>13</v>
+      <c r="D16" s="7"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="22"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1">
+      <c r="A17" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="C17" s="7">
         <v>1</v>
       </c>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>13</v>
+      <c r="D17" s="7"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="22"/>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1">
+      <c r="A18" s="18" t="s">
+        <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="C18" s="7">
         <v>1</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12" t="s">
-        <v>19</v>
+      <c r="D18" s="7"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1">
+      <c r="A19" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C19" s="7">
-        <v>2</v>
-      </c>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1">
       <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C20" s="7">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1">
       <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C21" s="7">
-        <v>2</v>
-      </c>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="22"/>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1">
       <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C22" s="7">
-        <v>2</v>
-      </c>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1">
       <c r="A23" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C23" s="7">
-        <v>2</v>
-      </c>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="22"/>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1">
       <c r="A24" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C24" s="7">
-        <v>2</v>
-      </c>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1">
       <c r="A25" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C25" s="7">
         <v>1</v>
       </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="D25" s="7"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1">
+      <c r="A26" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1</v>
+      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="22"/>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1">
+      <c r="A27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="7">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="22"/>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1">
+      <c r="A28" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="22"/>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1">
+      <c r="A29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="7">
+        <v>1</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1">
+      <c r="A30" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C30" s="7">
+        <v>1</v>
+      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" spans="1:6" s="2" customFormat="1">
+      <c r="A31" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C31" s="7">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="22"/>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1">
+      <c r="A32" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="21">
+        <v>2</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="22"/>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1">
+      <c r="A33" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="7">
-        <v>1</v>
-      </c>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="7">
-        <v>1</v>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="B33" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C28" s="7">
-        <v>2</v>
-      </c>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="7">
-        <v>3</v>
-      </c>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="7">
-        <v>1</v>
-      </c>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="7">
-        <v>1</v>
-      </c>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="C33" s="7">
         <v>2</v>
       </c>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="15" t="s">
-        <v>36</v>
+      <c r="D33" s="7"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="22"/>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1">
+      <c r="A34" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C34" s="7">
-        <v>1</v>
-      </c>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="15" t="s">
-        <v>36</v>
+        <v>2</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1">
+      <c r="A35" s="10" t="s">
+        <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>38</v>
+        <v>12</v>
       </c>
       <c r="C35" s="7">
         <v>2</v>
       </c>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="15" t="s">
-        <v>36</v>
+      <c r="D35" s="7"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1">
+      <c r="A36" s="14" t="s">
+        <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C36" s="7">
         <v>2</v>
       </c>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="7"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1">
       <c r="A37" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" s="7">
         <v>2</v>
       </c>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16" t="s">
-        <v>41</v>
+      <c r="D37" s="7"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="22"/>
+    </row>
+    <row r="38" spans="1:6" s="2" customFormat="1">
+      <c r="A38" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C38" s="7">
-        <v>1</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16" t="s">
-        <v>41</v>
+        <v>2</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1">
+      <c r="A39" s="15" t="s">
+        <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C39" s="7">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16" t="s">
-        <v>41</v>
+        <v>2</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="22"/>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1">
+      <c r="A40" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C40" s="7">
-        <v>3</v>
-      </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="16" t="s">
-        <v>41</v>
+        <v>2</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1">
+      <c r="A41" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C41" s="7">
-        <v>3</v>
-      </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="22"/>
+    </row>
+    <row r="42" spans="1:6" s="2" customFormat="1">
       <c r="A42" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C42" s="7">
         <v>2</v>
       </c>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
-        <v>48</v>
+      <c r="D42" s="7"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1">
+      <c r="A43" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="C43" s="7">
-        <v>2</v>
-      </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
-        <v>48</v>
+        <v>3</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="22"/>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1">
+      <c r="A44" s="9" t="s">
+        <v>0</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C44" s="7">
-        <v>2</v>
-      </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="18" t="s">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1">
+      <c r="A45" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="C45" s="7">
-        <v>1</v>
-      </c>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18" t="s">
-        <v>50</v>
+        <v>3</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="22"/>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1">
+      <c r="A46" s="16" t="s">
+        <v>41</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C46" s="7">
-        <v>1</v>
-      </c>
-      <c r="D46" s="4"/>
+        <v>3</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1">
+      <c r="A47" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="7">
+        <v>3</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="22"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1"/>
-  <conditionalFormatting sqref="C2:C46">
+  <autoFilter ref="A1:E1">
+    <filterColumn colId="3"/>
+  </autoFilter>
+  <sortState ref="A2:F47">
+    <sortCondition ref="C1"/>
+  </sortState>
+  <conditionalFormatting sqref="C2:D47">
     <cfRule type="iconSet" priority="1">
       <iconSet reverse="1">
         <cfvo type="percent" val="0"/>
@@ -1310,24 +1520,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating classes and documentation
Updating classes and documentation
</commit_message>
<xml_diff>
--- a/docs/Projeto.xlsx
+++ b/docs/Projeto.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="79">
   <si>
     <t>Basics</t>
   </si>
@@ -225,12 +225,6 @@
     <t>position, size</t>
   </si>
   <si>
-    <t>Escrita</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
     <t>Criar e herdar objetos, fazer merge de objetos, adicionar e remover eventos, parse JSON e converter para String</t>
   </si>
   <si>
@@ -249,10 +243,19 @@
     <t>id, size, path, file, isLoaded</t>
   </si>
   <si>
-    <t>Retorna o objeto Image, tamanho, get de largura e altura, se está carregado ou não, função de desenho padrão, clonar, serializar</t>
-  </si>
-  <si>
     <t>Clonar e serializar</t>
+  </si>
+  <si>
+    <t>red, green, blue, alpha</t>
+  </si>
+  <si>
+    <t>Formatar RGB, formatar RGBA, Clonar, Serializar</t>
+  </si>
+  <si>
+    <t>Retorna o objeto Image, tamanho, retorna largura e altura, se está carregado ou não, função de desenho padrão, clonar, serializar</t>
+  </si>
+  <si>
+    <t>id, name, size, unit</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -448,14 +451,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -769,31 +775,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="18" style="3" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="8"/>
-    <col min="4" max="4" width="32.140625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="104.7109375" style="5" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="3"/>
+    <col min="2" max="2" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="113.140625" style="5" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1">
+    <row r="1" spans="1:5" s="6" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>52</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="21" t="s">
         <v>54</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -802,38 +807,32 @@
       <c r="E1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="22">
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="F2" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="22">
         <v>1</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -842,18 +841,15 @@
       <c r="E3" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F3" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="22">
         <v>1</v>
       </c>
       <c r="D4" s="7" t="s">
@@ -862,18 +858,15 @@
       <c r="E4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="30">
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" ht="30">
       <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="22">
         <v>1</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -882,621 +875,576 @@
       <c r="E5" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1">
       <c r="A6" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="22">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F6" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="22">
         <v>1</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F7" s="22" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="2" customFormat="1">
+    <row r="8" spans="1:5" s="2" customFormat="1">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="22">
+        <v>1</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="20">
-        <v>1</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1">
       <c r="A9" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1">
       <c r="A10" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="2">
         <v>1</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="22"/>
-    </row>
-    <row r="11" spans="1:6" s="2" customFormat="1" ht="30">
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" ht="16.5" customHeight="1">
       <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="22">
         <v>1</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="22"/>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1">
       <c r="A12" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C12" s="7">
-        <v>1</v>
-      </c>
-      <c r="D12" s="7"/>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="20"/>
       <c r="E12" s="4"/>
-      <c r="F12" s="22"/>
-    </row>
-    <row r="13" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1">
       <c r="A13" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="2">
         <v>1</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="22"/>
-    </row>
-    <row r="14" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1">
       <c r="A14" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="2">
         <v>1</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="22"/>
-    </row>
-    <row r="15" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1">
       <c r="A15" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="7">
+      <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="22"/>
-    </row>
-    <row r="16" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1">
       <c r="A16" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="2">
         <v>1</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="22"/>
-    </row>
-    <row r="17" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1">
       <c r="A17" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="2">
         <v>1</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="22"/>
-    </row>
-    <row r="18" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1">
       <c r="A18" s="18" t="s">
         <v>50</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="2">
         <v>1</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="22"/>
-    </row>
-    <row r="19" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1">
       <c r="A19" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="2">
         <v>1</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="22"/>
-    </row>
-    <row r="20" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1">
       <c r="A20" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="2">
         <v>1</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="22"/>
-    </row>
-    <row r="21" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1">
       <c r="A21" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="2">
         <v>1</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="22"/>
-    </row>
-    <row r="22" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="22" spans="1:5" s="2" customFormat="1">
       <c r="A22" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="2">
         <v>1</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="22"/>
-    </row>
-    <row r="23" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1">
       <c r="A23" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="2">
         <v>1</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="22"/>
-    </row>
-    <row r="24" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1">
       <c r="A24" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="2">
         <v>1</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="22"/>
-    </row>
-    <row r="25" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1">
       <c r="A25" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="2">
         <v>1</v>
       </c>
       <c r="D25" s="7"/>
       <c r="E25" s="4"/>
-      <c r="F25" s="22"/>
-    </row>
-    <row r="26" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1">
       <c r="A26" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="2">
         <v>1</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="22"/>
-    </row>
-    <row r="27" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1">
       <c r="A27" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="7">
-        <v>1</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="22"/>
-    </row>
-    <row r="28" spans="1:6" s="2" customFormat="1">
+      <c r="C27" s="22">
+        <v>1</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1">
       <c r="A28" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="2">
         <v>1</v>
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="22"/>
-    </row>
-    <row r="29" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1">
       <c r="A29" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="2">
         <v>1</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="22"/>
-    </row>
-    <row r="30" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1">
       <c r="A30" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="2">
         <v>1</v>
       </c>
       <c r="D30" s="7"/>
       <c r="E30" s="4"/>
-      <c r="F30" s="22"/>
-    </row>
-    <row r="31" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1">
       <c r="A31" s="11" t="s">
         <v>13</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="7">
-        <v>1</v>
-      </c>
-      <c r="D31" s="7"/>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="E31" s="4"/>
-      <c r="F31" s="22"/>
-    </row>
-    <row r="32" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="32" spans="1:5" s="2" customFormat="1">
       <c r="A32" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="21">
+      <c r="C32" s="23">
         <v>2</v>
       </c>
       <c r="D32" s="7" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="4"/>
-      <c r="F32" s="22"/>
-    </row>
-    <row r="33" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1">
       <c r="A33" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="2">
         <v>2</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="4"/>
-      <c r="F33" s="22"/>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1">
       <c r="A34" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="7">
+      <c r="C34" s="2">
         <v>2</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="4"/>
-      <c r="F34" s="22"/>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1">
       <c r="A35" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="2">
         <v>2</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="4"/>
-      <c r="F35" s="22"/>
-    </row>
-    <row r="36" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1">
       <c r="A36" s="14" t="s">
         <v>32</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C36" s="2">
         <v>2</v>
       </c>
       <c r="D36" s="7"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="22"/>
-    </row>
-    <row r="37" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1">
       <c r="A37" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="7">
+      <c r="C37" s="2">
         <v>2</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="4"/>
-      <c r="F37" s="22"/>
-    </row>
-    <row r="38" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1">
       <c r="A38" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="7">
+      <c r="C38" s="2">
         <v>2</v>
       </c>
       <c r="D38" s="7"/>
       <c r="E38" s="4"/>
-      <c r="F38" s="22"/>
-    </row>
-    <row r="39" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1">
       <c r="A39" s="15" t="s">
         <v>36</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="7">
+      <c r="C39" s="2">
         <v>2</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="4"/>
-      <c r="F39" s="22"/>
-    </row>
-    <row r="40" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1">
       <c r="A40" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="7">
+      <c r="C40" s="2">
         <v>2</v>
       </c>
       <c r="D40" s="7"/>
       <c r="E40" s="4"/>
-      <c r="F40" s="22"/>
-    </row>
-    <row r="41" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1">
       <c r="A41" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="7">
+      <c r="C41" s="2">
         <v>2</v>
       </c>
       <c r="D41" s="7"/>
       <c r="E41" s="4"/>
-      <c r="F41" s="22"/>
-    </row>
-    <row r="42" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1">
       <c r="A42" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C42" s="7">
+      <c r="C42" s="2">
         <v>2</v>
       </c>
       <c r="D42" s="7"/>
       <c r="E42" s="4"/>
-      <c r="F42" s="22"/>
-    </row>
-    <row r="43" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1">
       <c r="A43" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="7">
+      <c r="C43" s="2">
         <v>3</v>
       </c>
       <c r="D43" s="7"/>
       <c r="E43" s="4"/>
-      <c r="F43" s="22"/>
-    </row>
-    <row r="44" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1">
       <c r="A44" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C44" s="7">
+      <c r="C44" s="2">
         <v>3</v>
       </c>
       <c r="D44" s="7"/>
       <c r="E44" s="4"/>
-      <c r="F44" s="22"/>
-    </row>
-    <row r="45" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1">
       <c r="A45" s="13" t="s">
         <v>27</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C45" s="7">
+      <c r="C45" s="2">
         <v>3</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="4"/>
-      <c r="F45" s="22"/>
-    </row>
-    <row r="46" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1">
       <c r="A46" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C46" s="7">
+      <c r="C46" s="2">
         <v>3</v>
       </c>
       <c r="D46" s="7"/>
       <c r="E46" s="4"/>
-      <c r="F46" s="22"/>
-    </row>
-    <row r="47" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1">
       <c r="A47" s="16" t="s">
         <v>41</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C47" s="7">
+      <c r="C47" s="2">
         <v>3</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="4"/>
-      <c r="F47" s="22"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1">

</xml_diff>

<commit_message>
Update Keyboard and Mouse events
Update Keyboard and Mouse events
</commit_message>
<xml_diff>
--- a/docs/Projeto.xlsx
+++ b/docs/Projeto.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafael\Projetos\HovinJS\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="90" windowWidth="14355" windowHeight="4680"/>
   </bookViews>
@@ -17,14 +12,14 @@
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$E$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Plan1!$A$1:$E$51</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="106">
   <si>
     <t>Basics</t>
   </si>
@@ -125,9 +120,6 @@
     <t>Game</t>
   </si>
   <si>
-    <t>Render</t>
-  </si>
-  <si>
     <t>Timer</t>
   </si>
   <si>
@@ -344,14 +336,14 @@
     <t>Criar por tamanho e ângulo, tamanho, normalizar, ângulo, rotação, ângulo entre dois vetores, normalizar e retornar novo</t>
   </si>
   <si>
-    <t>Screen</t>
+    <t>Viewport</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -619,7 +611,7 @@
     </a:clrScheme>
     <a:fontScheme name="Escritório">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -651,10 +643,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -686,7 +677,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -862,15 +852,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.28515625" style="17" customWidth="1"/>
     <col min="2" max="2" width="16.42578125" style="3" bestFit="1" customWidth="1"/>
@@ -880,41 +870,41 @@
     <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="6" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>54</v>
-      </c>
       <c r="D1" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1">
       <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C2" s="19">
         <v>1</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1">
       <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
@@ -925,13 +915,13 @@
         <v>1</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -942,13 +932,13 @@
         <v>1</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1">
       <c r="A5" s="7" t="s">
         <v>0</v>
       </c>
@@ -959,13 +949,13 @@
         <v>1</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1">
       <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
@@ -976,13 +966,13 @@
         <v>1</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1">
       <c r="A7" s="7" t="s">
         <v>0</v>
       </c>
@@ -993,30 +983,30 @@
         <v>1</v>
       </c>
       <c r="D7" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1">
       <c r="A8" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" s="19">
+        <v>1</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>68</v>
       </c>
-      <c r="C8" s="19">
-        <v>1</v>
-      </c>
-      <c r="D8" s="21" t="s">
+      <c r="E8" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -1027,11 +1017,11 @@
         <v>2</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A10" s="7" t="s">
         <v>0</v>
       </c>
@@ -1044,7 +1034,7 @@
       <c r="D10" s="21"/>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" s="2" customFormat="1" ht="16.5" hidden="1" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -1057,7 +1047,7 @@
       <c r="D11" s="21"/>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" s="2" customFormat="1">
       <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
@@ -1070,7 +1060,7 @@
       <c r="D12" s="21"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" s="2" customFormat="1">
       <c r="A13" s="11" t="s">
         <v>27</v>
       </c>
@@ -1083,7 +1073,7 @@
       <c r="D13" s="21"/>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A14" s="11" t="s">
         <v>27</v>
       </c>
@@ -1096,7 +1086,7 @@
       <c r="D14" s="21"/>
       <c r="E14" s="4"/>
     </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A15" s="11" t="s">
         <v>27</v>
       </c>
@@ -1109,7 +1099,7 @@
       <c r="D15" s="21"/>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A16" s="8" t="s">
         <v>9</v>
       </c>
@@ -1122,7 +1112,7 @@
       <c r="D16" s="21"/>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A17" s="8" t="s">
         <v>9</v>
       </c>
@@ -1135,46 +1125,46 @@
       <c r="D17" s="21"/>
       <c r="E17" s="4"/>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="2" customFormat="1">
       <c r="A18" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="20">
+        <v>105</v>
+      </c>
+      <c r="C18" s="19">
         <v>1</v>
       </c>
       <c r="D18" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E18" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1">
       <c r="A19" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="19">
         <v>1</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1">
       <c r="A20" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C20" s="2">
         <v>1</v>
@@ -1182,12 +1172,12 @@
       <c r="D20" s="21"/>
       <c r="E20" s="4"/>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" s="2" customFormat="1">
       <c r="A21" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C21" s="20">
         <v>1</v>
@@ -1195,99 +1185,99 @@
       <c r="D21" s="21"/>
       <c r="E21" s="4"/>
     </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A22" s="12" t="s">
         <v>32</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C22" s="20">
-        <v>1</v>
+        <v>54</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
       </c>
       <c r="D22" s="21"/>
       <c r="E22" s="4"/>
     </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12" t="s">
-        <v>32</v>
+    <row r="23" spans="1:5" s="2" customFormat="1">
+      <c r="A23" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="2">
-        <v>2</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C23" s="19">
+        <v>1</v>
+      </c>
+      <c r="D23" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1">
       <c r="A24" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="C24" s="19">
         <v>1</v>
       </c>
       <c r="D24" s="21" t="s">
-        <v>71</v>
+        <v>96</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1">
       <c r="A25" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="19">
-        <v>1</v>
-      </c>
-      <c r="D25" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
+      <c r="D25" s="21"/>
+      <c r="E25" s="4"/>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1">
       <c r="A26" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="19">
+        <v>1</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>100</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" hidden="1">
+      <c r="A27" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C26" s="2">
-        <v>1</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="4"/>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C27" s="19">
-        <v>1</v>
-      </c>
-      <c r="D27" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <v>3</v>
+      </c>
+      <c r="D27" s="21"/>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A28" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>44</v>
@@ -1298,25 +1288,25 @@
       <c r="D28" s="21"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="14" t="s">
-        <v>41</v>
+    <row r="29" spans="1:5" s="2" customFormat="1">
+      <c r="A29" s="16" t="s">
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C29" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D29" s="21"/>
       <c r="E29" s="4"/>
     </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" s="2" customFormat="1">
       <c r="A30" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>51</v>
+        <v>95</v>
       </c>
       <c r="C30" s="2">
         <v>1</v>
@@ -1324,22 +1314,22 @@
       <c r="D30" s="21"/>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="16" t="s">
-        <v>50</v>
+    <row r="31" spans="1:5" s="2" customFormat="1" hidden="1">
+      <c r="A31" s="13" t="s">
+        <v>35</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="C31" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="21"/>
       <c r="E31" s="4"/>
     </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A32" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>38</v>
@@ -1350,9 +1340,9 @@
       <c r="D32" s="21"/>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A33" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>39</v>
@@ -1363,12 +1353,12 @@
       <c r="D33" s="21"/>
       <c r="E33" s="4"/>
     </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>36</v>
+    <row r="34" spans="1:5" s="2" customFormat="1" hidden="1">
+      <c r="A34" s="15" t="s">
+        <v>47</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C34" s="2">
         <v>2</v>
@@ -1376,9 +1366,9 @@
       <c r="D34" s="21"/>
       <c r="E34" s="4"/>
     </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A35" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>46</v>
@@ -1389,12 +1379,12 @@
       <c r="D35" s="21"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" s="2" customFormat="1" hidden="1">
       <c r="A36" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C36" s="2">
         <v>2</v>
@@ -1402,212 +1392,216 @@
       <c r="D36" s="21"/>
       <c r="E36" s="4"/>
     </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="15" t="s">
-        <v>48</v>
+    <row r="37" spans="1:5" s="2" customFormat="1">
+      <c r="A37" s="10" t="s">
+        <v>19</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C37" s="2">
-        <v>2</v>
-      </c>
-      <c r="D37" s="21"/>
-      <c r="E37" s="4"/>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C37" s="19">
+        <v>1</v>
+      </c>
+      <c r="D37" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1">
       <c r="A38" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C38" s="19">
         <v>1</v>
       </c>
       <c r="D38" s="21" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1">
       <c r="A39" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="C39" s="19">
         <v>1</v>
       </c>
       <c r="D39" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E39" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1">
       <c r="A40" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>87</v>
+        <v>21</v>
       </c>
       <c r="C40" s="19">
         <v>1</v>
       </c>
       <c r="D40" s="21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1">
       <c r="A41" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C41" s="19">
         <v>1</v>
       </c>
       <c r="D41" s="21" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1">
       <c r="A42" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C42" s="19">
         <v>1</v>
       </c>
       <c r="D42" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="E42" s="4" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1">
       <c r="A43" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C43" s="19">
         <v>1</v>
       </c>
       <c r="D43" s="21" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1">
       <c r="A44" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C44" s="19">
         <v>1</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
-        <v>19</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1">
+      <c r="A45" s="9" t="s">
+        <v>13</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C45" s="19">
         <v>1</v>
       </c>
       <c r="D45" s="21" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1">
       <c r="A46" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C46" s="19">
         <v>1</v>
       </c>
       <c r="D46" s="21" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" s="2" customFormat="1">
       <c r="A47" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C47" s="19">
         <v>1</v>
       </c>
       <c r="D47" s="21" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1">
       <c r="A48" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>16</v>
+        <v>81</v>
       </c>
       <c r="C48" s="19">
         <v>1</v>
       </c>
       <c r="D48" s="21" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1">
       <c r="A49" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="C49" s="19">
         <v>1</v>
@@ -1616,62 +1610,45 @@
         <v>83</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" s="2" customFormat="1">
       <c r="A50" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="C50" s="19">
         <v>1</v>
       </c>
       <c r="D50" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1">
       <c r="A51" s="9" t="s">
         <v>13</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>76</v>
+        <v>18</v>
       </c>
       <c r="C51" s="19">
         <v>1</v>
       </c>
       <c r="D51" s="21" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C52" s="19">
-        <v>1</v>
-      </c>
-      <c r="D52" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:E52">
+  <autoFilter ref="A1:E51">
     <filterColumn colId="2">
       <filters>
         <filter val="1"/>
@@ -1681,8 +1658,8 @@
   <sortState ref="A2:E52">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="C2:D52">
-    <cfRule type="iconSet" priority="4">
+  <conditionalFormatting sqref="C2:D51">
+    <cfRule type="iconSet" priority="5">
       <iconSet reverse="1">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -1696,25 +1673,44 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1">
+        <v>37133.96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1668.64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3">
+        <f>SUM(A1:A2)</f>
+        <v>38802.6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>